<commit_message>
go model new runs
</commit_message>
<xml_diff>
--- a/Graphene Oxide/Data/Liu_2012_GO_male_large_1_tissues_dif_times.xlsx
+++ b/Graphene Oxide/Data/Liu_2012_GO_male_large_1_tissues_dif_times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eviepapakyriakopoulou/Documents/GitHub/PFAS_PBK_models/Graphene Oxide/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07458C0C-FC78-9E4C-8047-D1F66A569385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85BA7DA-B7F1-754D-A6F0-8CB623BF7640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="15">
   <si>
     <t>Tissue</t>
   </si>
@@ -581,7 +581,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -597,6 +597,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -954,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1518,13 +1521,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B32" s="4">
-        <v>2</v>
-      </c>
-      <c r="C32" s="6">
-        <v>1.9181034482758701</v>
+        <v>30</v>
+      </c>
+      <c r="C32" s="7">
+        <v>0.01</v>
       </c>
       <c r="D32" s="4">
         <v>1</v>
@@ -1538,10 +1541,10 @@
         <v>10</v>
       </c>
       <c r="B33" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C33" s="6">
-        <v>1.6163793103448301</v>
+        <v>1.9181034482758701</v>
       </c>
       <c r="D33" s="4">
         <v>1</v>
@@ -1555,10 +1558,10 @@
         <v>10</v>
       </c>
       <c r="B34" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C34" s="6">
-        <v>0.66810344827585699</v>
+        <v>1.6163793103448301</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
@@ -1572,10 +1575,10 @@
         <v>10</v>
       </c>
       <c r="B35" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C35" s="6">
-        <v>0.51724137931034497</v>
+        <v>0.66810344827585699</v>
       </c>
       <c r="D35" s="4">
         <v>1</v>
@@ -1589,10 +1592,10 @@
         <v>10</v>
       </c>
       <c r="B36" s="4">
-        <v>180</v>
+        <v>30</v>
       </c>
       <c r="C36" s="6">
-        <v>0.56034482758620396</v>
+        <v>0.51724137931034497</v>
       </c>
       <c r="D36" s="4">
         <v>1</v>
@@ -1603,13 +1606,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" s="4">
-        <v>2</v>
+        <v>180</v>
       </c>
       <c r="C37" s="6">
-        <v>0.26288602850924497</v>
+        <v>0.56034482758620396</v>
       </c>
       <c r="D37" s="4">
         <v>1</v>
@@ -1623,10 +1626,10 @@
         <v>11</v>
       </c>
       <c r="B38" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C38" s="6">
-        <v>0.93545938824607699</v>
+        <v>0.26288602850924497</v>
       </c>
       <c r="D38" s="4">
         <v>1</v>
@@ -1640,15 +1643,32 @@
         <v>11</v>
       </c>
       <c r="B39" s="4">
+        <v>10</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0.93545938824607699</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="4">
         <v>180</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C40" s="6">
         <v>0.15086206896552001</v>
       </c>
-      <c r="D39" s="4">
-        <v>1</v>
-      </c>
-      <c r="E39" s="4" t="s">
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>